<commit_message>
Améliorations sur conditions de stockage et date de naissance
</commit_message>
<xml_diff>
--- a/src/main/resources/CBSDfiles/patient/Démences BADN exemple.xlsx
+++ b/src/main/resources/CBSDfiles/patient/Démences BADN exemple.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="84">
   <si>
     <t>Nom</t>
   </si>
@@ -253,6 +253,21 @@
   </si>
   <si>
     <t>MYR</t>
+  </si>
+  <si>
+    <t>MARTIN</t>
+  </si>
+  <si>
+    <t>BERNARD</t>
+  </si>
+  <si>
+    <t>ANDRE</t>
+  </si>
+  <si>
+    <t>Marie</t>
+  </si>
+  <si>
+    <t>Jean</t>
   </si>
 </sst>
 </file>
@@ -262,7 +277,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,6 +307,12 @@
       <sz val="10"/>
       <color indexed="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -333,10 +354,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -422,10 +446,12 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Pourcentage 2" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -724,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC46"/>
+  <dimension ref="A1:AC41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:D15"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,9 +841,15 @@
       <c r="AC1" s="13"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
+      <c r="A2" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>82</v>
+      </c>
       <c r="D2" s="15" t="s">
         <v>24</v>
       </c>
@@ -878,9 +910,13 @@
       <c r="AC2" s="14"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
+      <c r="A3" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>83</v>
+      </c>
       <c r="D3" s="15">
         <v>14611</v>
       </c>
@@ -941,9 +977,9 @@
       <c r="AC3" s="14"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
         <v>24</v>
       </c>
@@ -988,7 +1024,7 @@
       </c>
       <c r="T4" s="19"/>
       <c r="U4" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V4" s="15" t="s">
         <v>33</v>
@@ -1004,9 +1040,9 @@
       <c r="AC4" s="14"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
         <v>24</v>
       </c>
@@ -1067,9 +1103,9 @@
       <c r="AC5" s="14"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="15">
         <v>18264</v>
       </c>
@@ -1114,7 +1150,7 @@
       </c>
       <c r="T6" s="19"/>
       <c r="U6" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V6" s="15" t="s">
         <v>33</v>
@@ -1130,9 +1166,9 @@
       <c r="AC6" s="14"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
         <v>24</v>
       </c>
@@ -1193,9 +1229,9 @@
       <c r="AC7" s="14"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="15">
         <v>21916</v>
       </c>
@@ -1256,9 +1292,9 @@
       <c r="AC8" s="14"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="15">
         <v>14611</v>
       </c>
@@ -1319,9 +1355,9 @@
       <c r="AC9" s="14"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="15">
         <v>18264</v>
       </c>
@@ -1366,7 +1402,7 @@
       </c>
       <c r="T10" s="19"/>
       <c r="U10" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V10" s="15" t="s">
         <v>33</v>
@@ -1382,9 +1418,9 @@
       <c r="AC10" s="14"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
         <v>24</v>
       </c>
@@ -1429,7 +1465,7 @@
       </c>
       <c r="T11" s="19"/>
       <c r="U11" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V11" s="15" t="s">
         <v>31</v>
@@ -1445,9 +1481,9 @@
       <c r="AC11" s="14"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="15">
         <v>21916</v>
       </c>
@@ -1492,7 +1528,7 @@
       </c>
       <c r="T12" s="19"/>
       <c r="U12" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V12" s="15" t="s">
         <v>33</v>
@@ -1508,9 +1544,9 @@
       <c r="AC12" s="14"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="15">
         <v>14611</v>
       </c>
@@ -1555,7 +1591,7 @@
       </c>
       <c r="T13" s="19"/>
       <c r="U13" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V13" s="15" t="s">
         <v>33</v>
@@ -1573,9 +1609,9 @@
       <c r="AC13" s="14"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="15">
         <v>18264</v>
       </c>
@@ -1620,7 +1656,7 @@
       </c>
       <c r="T14" s="19"/>
       <c r="U14" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V14" s="15" t="s">
         <v>33</v>
@@ -1636,9 +1672,9 @@
       <c r="AC14" s="14"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="15">
         <v>21916</v>
       </c>
@@ -1683,7 +1719,7 @@
       </c>
       <c r="T15" s="19"/>
       <c r="U15" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V15" s="15" t="s">
         <v>31</v>
@@ -1699,9 +1735,9 @@
       <c r="AC15" s="14"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="15">
         <v>14611</v>
       </c>
@@ -1746,7 +1782,7 @@
       </c>
       <c r="T16" s="19"/>
       <c r="U16" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V16" s="15" t="s">
         <v>33</v>
@@ -1762,9 +1798,9 @@
       <c r="AC16" s="14"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="15">
         <v>18264</v>
       </c>
@@ -1809,7 +1845,7 @@
       </c>
       <c r="T17" s="19"/>
       <c r="U17" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V17" s="15" t="s">
         <v>31</v>
@@ -1825,9 +1861,9 @@
       <c r="AC17" s="14"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
       <c r="D18" s="15">
         <v>21916</v>
       </c>
@@ -1872,7 +1908,7 @@
       </c>
       <c r="T18" s="19"/>
       <c r="U18" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V18" s="15" t="s">
         <v>33</v>
@@ -1888,9 +1924,9 @@
       <c r="AC18" s="14"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
       <c r="D19" s="15">
         <v>14611</v>
       </c>
@@ -1935,7 +1971,7 @@
       </c>
       <c r="T19" s="19"/>
       <c r="U19" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V19" s="15" t="s">
         <v>33</v>
@@ -1951,9 +1987,9 @@
       <c r="AC19" s="14"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
         <v>24</v>
       </c>
@@ -2014,9 +2050,9 @@
       <c r="AC20" s="14"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
       <c r="D21" s="15">
         <v>14611</v>
       </c>
@@ -2077,9 +2113,9 @@
       <c r="AC21" s="14"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
         <v>24</v>
       </c>
@@ -2124,7 +2160,7 @@
       </c>
       <c r="T22" s="19"/>
       <c r="U22" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V22" s="15" t="s">
         <v>51</v>
@@ -2140,9 +2176,9 @@
       <c r="AC22" s="14"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
       <c r="D23" s="15">
         <v>14611</v>
       </c>
@@ -2187,7 +2223,7 @@
       </c>
       <c r="T23" s="19"/>
       <c r="U23" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V23" s="15" t="s">
         <v>33</v>
@@ -2203,9 +2239,9 @@
       <c r="AC23" s="14"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
       <c r="D24" s="15">
         <v>18264</v>
       </c>
@@ -2250,7 +2286,7 @@
       </c>
       <c r="T24" s="19"/>
       <c r="U24" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V24" s="15" t="s">
         <v>33</v>
@@ -2266,9 +2302,9 @@
       <c r="AC24" s="14"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="15">
         <v>21916</v>
       </c>
@@ -2329,9 +2365,9 @@
       <c r="AC25" s="14"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="15">
         <v>14611</v>
       </c>
@@ -2376,7 +2412,7 @@
       </c>
       <c r="T26" s="19"/>
       <c r="U26" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V26" s="15" t="s">
         <v>33</v>
@@ -2392,9 +2428,9 @@
       <c r="AC26" s="14"/>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
       <c r="D27" s="15">
         <v>18264</v>
       </c>
@@ -2439,7 +2475,7 @@
       </c>
       <c r="T27" s="19"/>
       <c r="U27" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V27" s="15" t="s">
         <v>33</v>
@@ -2455,9 +2491,9 @@
       <c r="AC27" s="14"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
       <c r="D28" s="15">
         <v>21916</v>
       </c>
@@ -2518,9 +2554,9 @@
       <c r="AC28" s="14"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
       <c r="D29" s="15">
         <v>14611</v>
       </c>
@@ -2564,7 +2600,7 @@
         <v>29</v>
       </c>
       <c r="T29" s="26"/>
-      <c r="U29" s="25" t="s">
+      <c r="U29" s="18" t="s">
         <v>32</v>
       </c>
       <c r="V29" s="23" t="s">
@@ -2581,9 +2617,9 @@
       <c r="AC29" s="22"/>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
       <c r="D30" s="15">
         <v>18264</v>
       </c>
@@ -2628,7 +2664,7 @@
       </c>
       <c r="T30" s="19"/>
       <c r="U30" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V30" s="15" t="s">
         <v>33</v>
@@ -2644,9 +2680,9 @@
       <c r="AC30" s="14"/>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
       <c r="D31" s="15">
         <v>21916</v>
       </c>
@@ -2690,8 +2726,8 @@
         <v>29</v>
       </c>
       <c r="T31" s="26"/>
-      <c r="U31" s="25" t="s">
-        <v>30</v>
+      <c r="U31" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="V31" s="23" t="s">
         <v>33</v>
@@ -2707,9 +2743,9 @@
       <c r="AC31" s="22"/>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
       <c r="D32" s="15">
         <v>14611</v>
       </c>
@@ -2770,9 +2806,9 @@
       <c r="AC32" s="14"/>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
       <c r="D33" s="15">
         <v>18264</v>
       </c>
@@ -2817,7 +2853,7 @@
       </c>
       <c r="T33" s="19"/>
       <c r="U33" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V33" s="15" t="s">
         <v>33</v>
@@ -2833,9 +2869,9 @@
       <c r="AC33" s="14"/>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
       <c r="D34" s="15">
         <v>21916</v>
       </c>
@@ -2896,9 +2932,9 @@
       <c r="AC34" s="14"/>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
       <c r="D35" s="15">
         <v>14611</v>
       </c>
@@ -2959,9 +2995,9 @@
       <c r="AC35" s="14"/>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
       <c r="D36" s="15">
         <v>18264</v>
       </c>
@@ -3022,9 +3058,9 @@
       <c r="AC36" s="14"/>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
       <c r="D37" s="15">
         <v>21916</v>
       </c>
@@ -3085,9 +3121,9 @@
       <c r="AC37" s="14"/>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
       <c r="D38" s="15">
         <v>14611</v>
       </c>
@@ -3131,8 +3167,8 @@
         <v>29</v>
       </c>
       <c r="T38" s="26"/>
-      <c r="U38" s="25" t="s">
-        <v>30</v>
+      <c r="U38" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="V38" s="23" t="s">
         <v>33</v>
@@ -3148,9 +3184,9 @@
       <c r="AC38" s="22"/>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
       <c r="D39" s="15">
         <v>18264</v>
       </c>
@@ -3195,7 +3231,7 @@
       </c>
       <c r="T39" s="19"/>
       <c r="U39" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V39" s="15" t="s">
         <v>33</v>
@@ -3211,9 +3247,9 @@
       <c r="AC39" s="14"/>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
       <c r="D40" s="15">
         <v>21916</v>
       </c>
@@ -3258,7 +3294,7 @@
       </c>
       <c r="T40" s="19"/>
       <c r="U40" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V40" s="15" t="s">
         <v>33</v>
@@ -3274,9 +3310,9 @@
       <c r="AC40" s="14"/>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
       <c r="D41" s="15">
         <v>21916</v>
       </c>
@@ -3335,161 +3371,6 @@
       </c>
       <c r="AB41" s="15"/>
       <c r="AC41" s="14"/>
-    </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
-      <c r="O42" s="29"/>
-      <c r="P42" s="29"/>
-      <c r="Q42" s="29"/>
-      <c r="R42" s="29"/>
-      <c r="S42" s="29"/>
-      <c r="T42" s="29"/>
-      <c r="U42" s="29"/>
-      <c r="V42" s="29"/>
-      <c r="W42" s="29"/>
-      <c r="X42" s="29"/>
-      <c r="Y42" s="29"/>
-      <c r="Z42" s="29"/>
-      <c r="AA42" s="29"/>
-      <c r="AB42" s="29"/>
-      <c r="AC42" s="29"/>
-    </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="29"/>
-      <c r="N43" s="29"/>
-      <c r="O43" s="29"/>
-      <c r="P43" s="29"/>
-      <c r="Q43" s="29"/>
-      <c r="R43" s="29"/>
-      <c r="S43" s="29"/>
-      <c r="T43" s="29"/>
-      <c r="U43" s="29"/>
-      <c r="V43" s="29"/>
-      <c r="W43" s="29"/>
-      <c r="X43" s="29"/>
-      <c r="Y43" s="29"/>
-      <c r="Z43" s="29"/>
-      <c r="AA43" s="29"/>
-      <c r="AB43" s="29"/>
-      <c r="AC43" s="29"/>
-    </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="29"/>
-      <c r="N44" s="29"/>
-      <c r="O44" s="29"/>
-      <c r="P44" s="29"/>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="29"/>
-      <c r="S44" s="29"/>
-      <c r="T44" s="29"/>
-      <c r="U44" s="29"/>
-      <c r="V44" s="29"/>
-      <c r="W44" s="29"/>
-      <c r="X44" s="29"/>
-      <c r="Y44" s="29"/>
-      <c r="Z44" s="29"/>
-      <c r="AA44" s="29"/>
-      <c r="AB44" s="29"/>
-      <c r="AC44" s="29"/>
-    </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="29"/>
-      <c r="L45" s="29"/>
-      <c r="M45" s="29"/>
-      <c r="N45" s="29"/>
-      <c r="O45" s="29"/>
-      <c r="P45" s="29"/>
-      <c r="Q45" s="29"/>
-      <c r="R45" s="29"/>
-      <c r="S45" s="29"/>
-      <c r="T45" s="29"/>
-      <c r="U45" s="29"/>
-      <c r="V45" s="29"/>
-      <c r="W45" s="29"/>
-      <c r="X45" s="29"/>
-      <c r="Y45" s="29"/>
-      <c r="Z45" s="29"/>
-      <c r="AA45" s="29"/>
-      <c r="AB45" s="29"/>
-      <c r="AC45" s="29"/>
-    </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="29"/>
-      <c r="H46" s="29"/>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
-      <c r="K46" s="29"/>
-      <c r="L46" s="29"/>
-      <c r="M46" s="29"/>
-      <c r="N46" s="29"/>
-      <c r="O46" s="29"/>
-      <c r="P46" s="29"/>
-      <c r="Q46" s="29"/>
-      <c r="R46" s="29"/>
-      <c r="S46" s="29"/>
-      <c r="T46" s="29"/>
-      <c r="U46" s="29"/>
-      <c r="V46" s="29"/>
-      <c r="W46" s="29"/>
-      <c r="X46" s="29"/>
-      <c r="Y46" s="29"/>
-      <c r="Z46" s="29"/>
-      <c r="AA46" s="29"/>
-      <c r="AB46" s="29"/>
-      <c r="AC46" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout de noms et prénoms fictifs
</commit_message>
<xml_diff>
--- a/src/main/resources/CBSDfiles/patient/Démences BADN exemple.xlsx
+++ b/src/main/resources/CBSDfiles/patient/Démences BADN exemple.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="159">
   <si>
     <t>Nom</t>
   </si>
@@ -268,6 +268,231 @@
   </si>
   <si>
     <t>Jean</t>
+  </si>
+  <si>
+    <t>THOMAS</t>
+  </si>
+  <si>
+    <t>Michel</t>
+  </si>
+  <si>
+    <t>PETIT</t>
+  </si>
+  <si>
+    <t>Pierre</t>
+  </si>
+  <si>
+    <t>ROBERT</t>
+  </si>
+  <si>
+    <t>Philippe</t>
+  </si>
+  <si>
+    <t>RICHARD</t>
+  </si>
+  <si>
+    <t>Alain</t>
+  </si>
+  <si>
+    <t>DURAND</t>
+  </si>
+  <si>
+    <t>Nathalie</t>
+  </si>
+  <si>
+    <t>DUBOIS</t>
+  </si>
+  <si>
+    <t>Dominique</t>
+  </si>
+  <si>
+    <t>MOREAU</t>
+  </si>
+  <si>
+    <t>Nicolas</t>
+  </si>
+  <si>
+    <t>LAURENT</t>
+  </si>
+  <si>
+    <t>Isabelle</t>
+  </si>
+  <si>
+    <t>SIMON</t>
+  </si>
+  <si>
+    <t>Catherine</t>
+  </si>
+  <si>
+    <t>MICHEL</t>
+  </si>
+  <si>
+    <t>Monique</t>
+  </si>
+  <si>
+    <t>LEFEBVRE</t>
+  </si>
+  <si>
+    <t>Sylvie</t>
+  </si>
+  <si>
+    <t>LEROY</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>ROUX</t>
+  </si>
+  <si>
+    <t>Bernard</t>
+  </si>
+  <si>
+    <t>DAVID</t>
+  </si>
+  <si>
+    <t>Françoise</t>
+  </si>
+  <si>
+    <t>BERTRAND</t>
+  </si>
+  <si>
+    <t>Claude</t>
+  </si>
+  <si>
+    <t>MOREL</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>FOURNIER</t>
+  </si>
+  <si>
+    <t>Christophe</t>
+  </si>
+  <si>
+    <t>GIRARD</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>BONNET</t>
+  </si>
+  <si>
+    <t>André</t>
+  </si>
+  <si>
+    <t>DUPONT</t>
+  </si>
+  <si>
+    <t>Jacques</t>
+  </si>
+  <si>
+    <t>LAMBERT</t>
+  </si>
+  <si>
+    <t>Martine</t>
+  </si>
+  <si>
+    <t>FONTAINE</t>
+  </si>
+  <si>
+    <t>Gérard</t>
+  </si>
+  <si>
+    <t>ROUSSEAU</t>
+  </si>
+  <si>
+    <t>Jacqueline</t>
+  </si>
+  <si>
+    <t>VINCENT</t>
+  </si>
+  <si>
+    <t>Frédéric</t>
+  </si>
+  <si>
+    <t>MULLER</t>
+  </si>
+  <si>
+    <t>Éric</t>
+  </si>
+  <si>
+    <t>LEFEVRE</t>
+  </si>
+  <si>
+    <t>Laurent</t>
+  </si>
+  <si>
+    <t>FAURE</t>
+  </si>
+  <si>
+    <t>Julien</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>MERCIER</t>
+  </si>
+  <si>
+    <t>Stéphane</t>
+  </si>
+  <si>
+    <t>BLANC</t>
+  </si>
+  <si>
+    <t>Sébastien</t>
+  </si>
+  <si>
+    <t>GUERIN</t>
+  </si>
+  <si>
+    <t>Anne</t>
+  </si>
+  <si>
+    <t>BOYER</t>
+  </si>
+  <si>
+    <t>Pascal</t>
+  </si>
+  <si>
+    <t>GARNIER</t>
+  </si>
+  <si>
+    <t>Christine</t>
+  </si>
+  <si>
+    <t>CHEVALIER</t>
+  </si>
+  <si>
+    <t>Nicole</t>
+  </si>
+  <si>
+    <t>FRANCOIS</t>
+  </si>
+  <si>
+    <t>Thierry</t>
+  </si>
+  <si>
+    <t>LEGRAND</t>
+  </si>
+  <si>
+    <t>Olivier</t>
+  </si>
+  <si>
+    <t>GAUTHIER</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>GARCIA</t>
+  </si>
+  <si>
+    <t>Alexandre</t>
   </si>
 </sst>
 </file>
@@ -753,11 +978,14 @@
   <dimension ref="A1:AC41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -896,7 +1124,7 @@
       <c r="U2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="V2" s="18" t="s">
         <v>31</v>
       </c>
       <c r="W2" s="16"/>
@@ -963,7 +1191,7 @@
       <c r="U3" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="V3" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W3" s="16"/>
@@ -977,9 +1205,13 @@
       <c r="AC3" s="14"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="15" t="s">
+        <v>84</v>
+      </c>
       <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="C4" s="15" t="s">
+        <v>85</v>
+      </c>
       <c r="D4" s="15" t="s">
         <v>24</v>
       </c>
@@ -1026,7 +1258,7 @@
       <c r="U4" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V4" s="15" t="s">
+      <c r="V4" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W4" s="16"/>
@@ -1040,9 +1272,13 @@
       <c r="AC4" s="14"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="15" t="s">
+        <v>86</v>
+      </c>
       <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+      <c r="C5" s="15" t="s">
+        <v>87</v>
+      </c>
       <c r="D5" s="15" t="s">
         <v>24</v>
       </c>
@@ -1089,7 +1325,7 @@
       <c r="U5" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V5" s="15" t="s">
+      <c r="V5" s="18" t="s">
         <v>31</v>
       </c>
       <c r="W5" s="16"/>
@@ -1103,9 +1339,13 @@
       <c r="AC5" s="14"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="15" t="s">
+        <v>88</v>
+      </c>
       <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
+      <c r="C6" s="15" t="s">
+        <v>89</v>
+      </c>
       <c r="D6" s="15">
         <v>18264</v>
       </c>
@@ -1152,7 +1392,7 @@
       <c r="U6" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V6" s="15" t="s">
+      <c r="V6" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W6" s="16"/>
@@ -1166,9 +1406,13 @@
       <c r="AC6" s="14"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+      <c r="A7" s="15" t="s">
+        <v>90</v>
+      </c>
       <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
+      <c r="C7" s="15" t="s">
+        <v>91</v>
+      </c>
       <c r="D7" s="15" t="s">
         <v>24</v>
       </c>
@@ -1215,7 +1459,7 @@
       <c r="U7" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V7" s="15" t="s">
+      <c r="V7" s="18" t="s">
         <v>31</v>
       </c>
       <c r="W7" s="16"/>
@@ -1229,9 +1473,13 @@
       <c r="AC7" s="14"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="15" t="s">
+        <v>92</v>
+      </c>
       <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
+      <c r="C8" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="D8" s="15">
         <v>21916</v>
       </c>
@@ -1278,7 +1526,7 @@
       <c r="U8" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="V8" s="15" t="s">
+      <c r="V8" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W8" s="16"/>
@@ -1292,9 +1540,13 @@
       <c r="AC8" s="14"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
+      <c r="A9" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
+      <c r="C9" s="15" t="s">
+        <v>95</v>
+      </c>
       <c r="D9" s="15">
         <v>14611</v>
       </c>
@@ -1341,7 +1593,7 @@
       <c r="U9" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V9" s="15" t="s">
+      <c r="V9" s="18" t="s">
         <v>31</v>
       </c>
       <c r="W9" s="16"/>
@@ -1355,9 +1607,13 @@
       <c r="AC9" s="14"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
+      <c r="A10" s="15" t="s">
+        <v>96</v>
+      </c>
       <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
+      <c r="C10" s="15" t="s">
+        <v>97</v>
+      </c>
       <c r="D10" s="15">
         <v>18264</v>
       </c>
@@ -1404,7 +1660,7 @@
       <c r="U10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V10" s="15" t="s">
+      <c r="V10" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W10" s="16"/>
@@ -1418,9 +1674,13 @@
       <c r="AC10" s="14"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
+      <c r="A11" s="15" t="s">
+        <v>98</v>
+      </c>
       <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
+      <c r="C11" s="15" t="s">
+        <v>99</v>
+      </c>
       <c r="D11" s="15" t="s">
         <v>24</v>
       </c>
@@ -1467,7 +1727,7 @@
       <c r="U11" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="V11" s="15" t="s">
+      <c r="V11" s="18" t="s">
         <v>31</v>
       </c>
       <c r="W11" s="16"/>
@@ -1481,9 +1741,13 @@
       <c r="AC11" s="14"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
+      <c r="A12" s="15" t="s">
+        <v>100</v>
+      </c>
       <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
+      <c r="C12" s="15" t="s">
+        <v>101</v>
+      </c>
       <c r="D12" s="15">
         <v>21916</v>
       </c>
@@ -1530,7 +1794,7 @@
       <c r="U12" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="V12" s="15" t="s">
+      <c r="V12" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W12" s="16"/>
@@ -1544,9 +1808,13 @@
       <c r="AC12" s="14"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
+      <c r="A13" s="15" t="s">
+        <v>102</v>
+      </c>
       <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
+      <c r="C13" s="15" t="s">
+        <v>103</v>
+      </c>
       <c r="D13" s="15">
         <v>14611</v>
       </c>
@@ -1593,7 +1861,7 @@
       <c r="U13" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="V13" s="15" t="s">
+      <c r="V13" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W13" s="16"/>
@@ -1609,9 +1877,13 @@
       <c r="AC13" s="14"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
+      <c r="A14" s="15" t="s">
+        <v>104</v>
+      </c>
       <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
+      <c r="C14" s="15" t="s">
+        <v>105</v>
+      </c>
       <c r="D14" s="15">
         <v>18264</v>
       </c>
@@ -1658,7 +1930,7 @@
       <c r="U14" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="V14" s="15" t="s">
+      <c r="V14" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W14" s="16"/>
@@ -1672,9 +1944,13 @@
       <c r="AC14" s="14"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
+      <c r="A15" s="15" t="s">
+        <v>106</v>
+      </c>
       <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
+      <c r="C15" s="15" t="s">
+        <v>107</v>
+      </c>
       <c r="D15" s="15">
         <v>21916</v>
       </c>
@@ -1721,7 +1997,7 @@
       <c r="U15" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V15" s="15" t="s">
+      <c r="V15" s="18" t="s">
         <v>31</v>
       </c>
       <c r="W15" s="16"/>
@@ -1735,9 +2011,13 @@
       <c r="AC15" s="14"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
+      <c r="A16" s="15" t="s">
+        <v>108</v>
+      </c>
       <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
+      <c r="C16" s="15" t="s">
+        <v>109</v>
+      </c>
       <c r="D16" s="15">
         <v>14611</v>
       </c>
@@ -1784,7 +2064,7 @@
       <c r="U16" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V16" s="15" t="s">
+      <c r="V16" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W16" s="16"/>
@@ -1798,9 +2078,13 @@
       <c r="AC16" s="14"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
+      <c r="A17" s="15" t="s">
+        <v>110</v>
+      </c>
       <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
+      <c r="C17" s="15" t="s">
+        <v>111</v>
+      </c>
       <c r="D17" s="15">
         <v>18264</v>
       </c>
@@ -1847,7 +2131,7 @@
       <c r="U17" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="V17" s="15" t="s">
+      <c r="V17" s="18" t="s">
         <v>31</v>
       </c>
       <c r="W17" s="16"/>
@@ -1861,9 +2145,13 @@
       <c r="AC17" s="14"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
+      <c r="A18" s="15" t="s">
+        <v>112</v>
+      </c>
       <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
+      <c r="C18" s="15" t="s">
+        <v>113</v>
+      </c>
       <c r="D18" s="15">
         <v>21916</v>
       </c>
@@ -1910,7 +2198,7 @@
       <c r="U18" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V18" s="15" t="s">
+      <c r="V18" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W18" s="16"/>
@@ -1924,9 +2212,13 @@
       <c r="AC18" s="14"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
+      <c r="A19" s="15" t="s">
+        <v>114</v>
+      </c>
       <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
+      <c r="C19" s="15" t="s">
+        <v>115</v>
+      </c>
       <c r="D19" s="15">
         <v>14611</v>
       </c>
@@ -1973,7 +2265,7 @@
       <c r="U19" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V19" s="15" t="s">
+      <c r="V19" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W19" s="16"/>
@@ -1987,9 +2279,13 @@
       <c r="AC19" s="14"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
+      <c r="A20" s="15" t="s">
+        <v>116</v>
+      </c>
       <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
+      <c r="C20" s="15" t="s">
+        <v>117</v>
+      </c>
       <c r="D20" s="15" t="s">
         <v>24</v>
       </c>
@@ -2036,7 +2332,7 @@
       <c r="U20" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V20" s="15" t="s">
+      <c r="V20" s="18" t="s">
         <v>31</v>
       </c>
       <c r="W20" s="16"/>
@@ -2050,9 +2346,13 @@
       <c r="AC20" s="14"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
+      <c r="A21" s="15" t="s">
+        <v>118</v>
+      </c>
       <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
+      <c r="C21" s="15" t="s">
+        <v>119</v>
+      </c>
       <c r="D21" s="15">
         <v>14611</v>
       </c>
@@ -2099,7 +2399,7 @@
       <c r="U21" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V21" s="15" t="s">
+      <c r="V21" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W21" s="16"/>
@@ -2113,9 +2413,13 @@
       <c r="AC21" s="14"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
+      <c r="A22" s="15" t="s">
+        <v>120</v>
+      </c>
       <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
+      <c r="C22" s="15" t="s">
+        <v>121</v>
+      </c>
       <c r="D22" s="15" t="s">
         <v>24</v>
       </c>
@@ -2162,7 +2466,7 @@
       <c r="U22" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V22" s="15" t="s">
+      <c r="V22" s="18" t="s">
         <v>51</v>
       </c>
       <c r="W22" s="16"/>
@@ -2176,9 +2480,13 @@
       <c r="AC22" s="14"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
+      <c r="A23" s="15" t="s">
+        <v>122</v>
+      </c>
       <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
+      <c r="C23" s="15" t="s">
+        <v>123</v>
+      </c>
       <c r="D23" s="15">
         <v>14611</v>
       </c>
@@ -2225,7 +2533,7 @@
       <c r="U23" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V23" s="15" t="s">
+      <c r="V23" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W23" s="16"/>
@@ -2239,9 +2547,13 @@
       <c r="AC23" s="14"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
+      <c r="A24" s="15" t="s">
+        <v>124</v>
+      </c>
       <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
+      <c r="C24" s="15" t="s">
+        <v>125</v>
+      </c>
       <c r="D24" s="15">
         <v>18264</v>
       </c>
@@ -2288,7 +2600,7 @@
       <c r="U24" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="V24" s="15" t="s">
+      <c r="V24" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W24" s="16"/>
@@ -2302,9 +2614,13 @@
       <c r="AC24" s="14"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
+      <c r="A25" s="15" t="s">
+        <v>126</v>
+      </c>
       <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
+      <c r="C25" s="15" t="s">
+        <v>127</v>
+      </c>
       <c r="D25" s="15">
         <v>21916</v>
       </c>
@@ -2351,7 +2667,7 @@
       <c r="U25" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V25" s="15" t="s">
+      <c r="V25" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W25" s="16"/>
@@ -2365,9 +2681,13 @@
       <c r="AC25" s="14"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
+      <c r="A26" s="15" t="s">
+        <v>128</v>
+      </c>
       <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
+      <c r="C26" s="15" t="s">
+        <v>129</v>
+      </c>
       <c r="D26" s="15">
         <v>14611</v>
       </c>
@@ -2414,7 +2734,7 @@
       <c r="U26" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="V26" s="15" t="s">
+      <c r="V26" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W26" s="16"/>
@@ -2428,9 +2748,13 @@
       <c r="AC26" s="14"/>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
+      <c r="A27" s="15" t="s">
+        <v>130</v>
+      </c>
       <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
+      <c r="C27" s="15" t="s">
+        <v>131</v>
+      </c>
       <c r="D27" s="15">
         <v>18264</v>
       </c>
@@ -2477,7 +2801,7 @@
       <c r="U27" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V27" s="15" t="s">
+      <c r="V27" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W27" s="16"/>
@@ -2491,9 +2815,13 @@
       <c r="AC27" s="14"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
+      <c r="A28" s="15" t="s">
+        <v>132</v>
+      </c>
       <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
+      <c r="C28" s="15" t="s">
+        <v>133</v>
+      </c>
       <c r="D28" s="15">
         <v>21916</v>
       </c>
@@ -2540,7 +2868,7 @@
       <c r="U28" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V28" s="15" t="s">
+      <c r="V28" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W28" s="16"/>
@@ -2554,9 +2882,13 @@
       <c r="AC28" s="14"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
+      <c r="A29" s="15" t="s">
+        <v>134</v>
+      </c>
       <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
+      <c r="C29" s="15" t="s">
+        <v>135</v>
+      </c>
       <c r="D29" s="15">
         <v>14611</v>
       </c>
@@ -2603,7 +2935,7 @@
       <c r="U29" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V29" s="23" t="s">
+      <c r="V29" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W29" s="24"/>
@@ -2617,9 +2949,13 @@
       <c r="AC29" s="22"/>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
+      <c r="A30" s="15" t="s">
+        <v>136</v>
+      </c>
       <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
+      <c r="C30" s="15" t="s">
+        <v>137</v>
+      </c>
       <c r="D30" s="15">
         <v>18264</v>
       </c>
@@ -2666,7 +3002,7 @@
       <c r="U30" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V30" s="15" t="s">
+      <c r="V30" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W30" s="16"/>
@@ -2680,9 +3016,13 @@
       <c r="AC30" s="14"/>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
+      <c r="A31" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
+      <c r="C31" s="15" t="s">
+        <v>138</v>
+      </c>
       <c r="D31" s="15">
         <v>21916</v>
       </c>
@@ -2729,7 +3069,7 @@
       <c r="U31" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V31" s="23" t="s">
+      <c r="V31" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W31" s="24"/>
@@ -2743,9 +3083,13 @@
       <c r="AC31" s="22"/>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
+      <c r="A32" s="15" t="s">
+        <v>139</v>
+      </c>
       <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
+      <c r="C32" s="15" t="s">
+        <v>140</v>
+      </c>
       <c r="D32" s="15">
         <v>14611</v>
       </c>
@@ -2792,7 +3136,7 @@
       <c r="U32" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V32" s="15" t="s">
+      <c r="V32" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W32" s="16"/>
@@ -2806,9 +3150,13 @@
       <c r="AC32" s="14"/>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
+      <c r="A33" s="15" t="s">
+        <v>141</v>
+      </c>
       <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
+      <c r="C33" s="15" t="s">
+        <v>142</v>
+      </c>
       <c r="D33" s="15">
         <v>18264</v>
       </c>
@@ -2855,7 +3203,7 @@
       <c r="U33" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V33" s="15" t="s">
+      <c r="V33" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W33" s="16"/>
@@ -2869,9 +3217,13 @@
       <c r="AC33" s="14"/>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
+      <c r="A34" s="15" t="s">
+        <v>143</v>
+      </c>
       <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
+      <c r="C34" s="15" t="s">
+        <v>144</v>
+      </c>
       <c r="D34" s="15">
         <v>21916</v>
       </c>
@@ -2918,7 +3270,7 @@
       <c r="U34" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="V34" s="15" t="s">
+      <c r="V34" s="18" t="s">
         <v>51</v>
       </c>
       <c r="W34" s="16"/>
@@ -2932,9 +3284,13 @@
       <c r="AC34" s="14"/>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
+      <c r="A35" s="15" t="s">
+        <v>145</v>
+      </c>
       <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
+      <c r="C35" s="15" t="s">
+        <v>146</v>
+      </c>
       <c r="D35" s="15">
         <v>14611</v>
       </c>
@@ -2981,7 +3337,7 @@
       <c r="U35" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V35" s="15" t="s">
+      <c r="V35" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W35" s="16"/>
@@ -2995,9 +3351,13 @@
       <c r="AC35" s="14"/>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
+      <c r="A36" s="15" t="s">
+        <v>147</v>
+      </c>
       <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
+      <c r="C36" s="15" t="s">
+        <v>148</v>
+      </c>
       <c r="D36" s="15">
         <v>18264</v>
       </c>
@@ -3044,7 +3404,7 @@
       <c r="U36" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="V36" s="15" t="s">
+      <c r="V36" s="18" t="s">
         <v>31</v>
       </c>
       <c r="W36" s="16"/>
@@ -3058,9 +3418,13 @@
       <c r="AC36" s="14"/>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
+      <c r="A37" s="15" t="s">
+        <v>149</v>
+      </c>
       <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
+      <c r="C37" s="15" t="s">
+        <v>150</v>
+      </c>
       <c r="D37" s="15">
         <v>21916</v>
       </c>
@@ -3107,7 +3471,7 @@
       <c r="U37" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="V37" s="15" t="s">
+      <c r="V37" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W37" s="16"/>
@@ -3121,9 +3485,13 @@
       <c r="AC37" s="14"/>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
+      <c r="A38" s="15" t="s">
+        <v>151</v>
+      </c>
       <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
+      <c r="C38" s="15" t="s">
+        <v>152</v>
+      </c>
       <c r="D38" s="15">
         <v>14611</v>
       </c>
@@ -3170,7 +3538,7 @@
       <c r="U38" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V38" s="23" t="s">
+      <c r="V38" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W38" s="24"/>
@@ -3184,9 +3552,13 @@
       <c r="AC38" s="22"/>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
+      <c r="A39" s="15" t="s">
+        <v>153</v>
+      </c>
       <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
+      <c r="C39" s="15" t="s">
+        <v>154</v>
+      </c>
       <c r="D39" s="15">
         <v>18264</v>
       </c>
@@ -3233,7 +3605,7 @@
       <c r="U39" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V39" s="15" t="s">
+      <c r="V39" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W39" s="16"/>
@@ -3247,9 +3619,13 @@
       <c r="AC39" s="14"/>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
+      <c r="A40" s="15" t="s">
+        <v>155</v>
+      </c>
       <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
+      <c r="C40" s="15" t="s">
+        <v>156</v>
+      </c>
       <c r="D40" s="15">
         <v>21916</v>
       </c>
@@ -3296,7 +3672,7 @@
       <c r="U40" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V40" s="15" t="s">
+      <c r="V40" s="18" t="s">
         <v>33</v>
       </c>
       <c r="W40" s="16"/>
@@ -3310,9 +3686,13 @@
       <c r="AC40" s="14"/>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
+      <c r="A41" s="15" t="s">
+        <v>157</v>
+      </c>
       <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
+      <c r="C41" s="15" t="s">
+        <v>158</v>
+      </c>
       <c r="D41" s="15">
         <v>21916</v>
       </c>
@@ -3357,7 +3737,7 @@
       <c r="U41" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V41" s="15" t="s">
+      <c r="V41" s="18" t="s">
         <v>31</v>
       </c>
       <c r="W41" s="16"/>

</xml_diff>